<commit_message>
Driver Charge Calculation and Fiscal Year Print in this commit
</commit_message>
<xml_diff>
--- a/App_Templates/cs_Template.xlsx
+++ b/App_Templates/cs_Template.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="-15" yWindow="4125" windowWidth="20520" windowHeight="4170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CS" sheetId="1" r:id="rId1"/>
+    <sheet name="CSN" sheetId="2" r:id="rId2"/>
+    <sheet name="CALC" sheetId="3" r:id="rId3"/>
+    <sheet name="IM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>COST SHEET</t>
   </si>
@@ -32,17 +35,126 @@
   </si>
   <si>
     <t>Particulars</t>
+  </si>
+  <si>
+    <t>Table Column 1 formula</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>Cost(W/o Incentive)</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Export Incentive</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>Margin rate W/o Incentive</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Table Column 2 formula</t>
+  </si>
+  <si>
+    <t>Revenue Calculation</t>
+  </si>
+  <si>
+    <t>Todate cost booked(W/o Exch.Vari)</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Proportionate revenue</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>Invoices raised</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>Short/Excess(-) Revenue</t>
+  </si>
+  <si>
+    <t>KK</t>
+  </si>
+  <si>
+    <t>Table Column 3 formula</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Prop. Contribution</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>Expo. Incentive booked</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>Exch. vari. on invoices</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>OO</t>
+  </si>
+  <si>
+    <t>Diff.</t>
+  </si>
+  <si>
+    <t>pp</t>
+  </si>
+  <si>
+    <t>Figures In Lakh</t>
+  </si>
+  <si>
+    <t>INPUT METHOD CALC.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,16 +216,370 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9.35"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -147,12 +613,189 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="27" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -180,10 +823,129 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="32" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="54">
+    <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="25" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="29" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="33" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="37" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="41" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="22" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="26" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="30" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="34" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="38" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="42" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="23" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="27" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="31" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="35" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="39" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="43" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="24" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="28" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="32" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="36" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="40" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="9" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="13" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="15" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="48"/>
+    <cellStyle name="Comma 3" xfId="50"/>
+    <cellStyle name="Comma 4" xfId="45"/>
+    <cellStyle name="Comma 5" xfId="53"/>
+    <cellStyle name="Comma 6" xfId="52"/>
+    <cellStyle name="Explanatory Text" xfId="18" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="8" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="5" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="6" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="7" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink 2" xfId="47"/>
+    <cellStyle name="Input" xfId="11" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="14" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="10" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="44"/>
+    <cellStyle name="Normal 3" xfId="49"/>
+    <cellStyle name="Normal 4" xfId="51"/>
+    <cellStyle name="Normal 7" xfId="46"/>
+    <cellStyle name="Note" xfId="17" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="12" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -484,11 +1246,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -499,12 +1261,12 @@
     <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -515,7 +1277,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
@@ -526,15 +1288,15 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
     </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -553,7 +1315,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="4"/>
@@ -572,4 +1334,640 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="G1" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="32">
+        <f>F1/100000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="32">
+        <f t="shared" ref="H2:H4" si="0">F2/100000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="13"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="13"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="13"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="13"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="13"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="13"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="13"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="13"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="13"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="13"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="16">
+        <f>IF(CS!G2="DOMESTIC",CSN!B11,CSN!B11-CSN!H4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="20">
+        <f>D3-CSN!B12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="21">
+        <f>CSN!B17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="16">
+        <f>CSN!B12+CSN!B17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="23" t="e">
+        <f>(D6-D5)/D3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="25">
+        <f>(CSN!H1-CSN!H2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="26" t="e">
+        <f>D11/D4*D3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="16">
+        <f>-CSN!B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="31" t="e">
+        <f>D12-D13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="29" t="e">
+        <f>D13*D7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="20">
+        <f>CSN!B18+CSN!B20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="20">
+        <f>-CSN!H2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="26" t="e">
+        <f>D17+D18+D19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="26" t="e">
+        <f>CSN!H3-CALC!D20</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="30"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="39">
+        <f>CALC!D3</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="35">
+        <f>CALC!D11</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="35"/>
+      <c r="F2" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="38" t="e">
+        <f>+B6*D3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="41">
+        <f>CALC!D4</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="35" t="e">
+        <f>CALC!D12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="38">
+        <f>CALC!D18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="42">
+        <f>CALC!D5</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="35">
+        <f>CALC!D13</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="35"/>
+      <c r="F4" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="38">
+        <f>CALC!D19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="39">
+        <f>CALC!D6</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="35" t="e">
+        <f>+D3-D4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="38" t="e">
+        <f>SUM(G2:G4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="43" t="e">
+        <f>+(B5-B4)/B2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="38" t="e">
+        <f>+G5-CSN!H3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>